<commit_message>
reference table created (must be re-run after removing errors!)
</commit_message>
<xml_diff>
--- a/inst/COMPILATION/reference_correction_subtitutions.xlsx
+++ b/inst/COMPILATION/reference_correction_subtitutions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNI\4. DOCTORADO\99. OTROS\2021_10_07 AFLIBER 2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNI\4. DOCTORADO\99. OTROS\2021_10_07 AFLIBER 2.0\AFLIBER_update\inst\COMPILATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A50916-5134-4BEC-B2A1-D2FDF2087DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759CEF1A-5097-4F93-A898-629437922135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{BFBE1423-48B3-41EF-9F48-2F6DFDC4ECE4}"/>
   </bookViews>
@@ -543,10 +543,10 @@
     <t>FAME (2011), Aparicio &amp; Silvestre (1987), Martínez Azorín et al. (2007)</t>
   </si>
   <si>
-    <t>Flora-on</t>
-  </si>
-  <si>
     <t>FloraOn</t>
+  </si>
+  <si>
+    <t>Flora-On: Flora de Portugal Interactiva. Sociedade Portuguesa de Botânica. www.flora-on.pt. Last accessed February, 2025.</t>
   </si>
 </sst>
 </file>
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB90C8D-81B1-481E-87E5-768B5E19E5D4}">
   <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,10 +1905,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>148</v>
+      </c>
+      <c r="B87" t="s">
         <v>149</v>
-      </c>
-      <c r="B87" t="s">
-        <v>148</v>
       </c>
       <c r="C87" t="s">
         <v>68</v>

</xml_diff>